<commit_message>
cambio en continuar compra
</commit_message>
<xml_diff>
--- a/resultados_scraping.xlsx
+++ b/resultados_scraping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,379 +535,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>15643401</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Llega mañana, 17 de jun.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>17/06/2025</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>110037565</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Llega mañana, 17 de jun.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>17/06/2025</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>138124130</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Llega entre el lunes 30 de jun y viernes 04 de jul.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>30/06/2025</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>17287672</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 18 de jun.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>17127319</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 18 de jun.</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>$ 4.990</t>
-        </is>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>15784952</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>$ 10.990</t>
-        </is>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>139603723</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>$ 4.990</t>
-        </is>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>7001702</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>$ 18.990</t>
-        </is>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>17243432</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 18 de jun.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Funciones para verificar acciones
</commit_message>
<xml_diff>
--- a/resultados_scraping.xlsx
+++ b/resultados_scraping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16/06/2025</t>
+          <t>17/06/2025</t>
         </is>
       </c>
       <c r="C2" t="b">
@@ -509,7 +509,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Llega entre el viernes 04 y jueves 10 de jul.</t>
+          <t>Llega entre el lunes 07 y viernes 11 de jul.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -526,12 +526,12 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>04/07/2025</t>
+          <t>07/07/2025</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>10/07/2025</t>
+          <t>11/07/2025</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16/06/2025</t>
+          <t>17/06/2025</t>
         </is>
       </c>
       <c r="C3" t="b">
@@ -554,7 +554,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Llega mañana, 17 de jun.</t>
+          <t>Llega mañana, 18 de jun.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -570,343 +570,11 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>17/06/2025</t>
+          <t>18/06/2025</t>
         </is>
       </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>110037565</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Llega mañana, 17 de jun.</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>17/06/2025</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>138124130</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Llega entre el lunes 30 de jun y viernes 04 de jul.</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>30/06/2025</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>04/07/2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>17287672</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 18 de jun.</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>17127319</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>$ 4.990</t>
-        </is>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>15784952</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>$ 10.990</t>
-        </is>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>139603723</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Llega el jueves 19 de jun.</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>$ 4.990</t>
-        </is>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>19/06/2025</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>7001702</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 02 de jul.</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>$ 18.990</t>
-        </is>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>02/07/2025</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>17243432</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>16/06/2025</t>
-        </is>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Llega el miércoles 18 de jun.</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>$ 3.990</t>
-        </is>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>18/06/2025</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>